<commit_message>
Removing extra SNPs from LFAR and WRAP markers in supplementary table and removing extra supplementary table csv.
</commit_message>
<xml_diff>
--- a/inputs/ChinookFullPanelLociTable_Feb2024Updated.xlsx
+++ b/inputs/ChinookFullPanelLociTable_Feb2024Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellen/Genetics_Lab_Data/DataAnalysis/california-chinook-microhaps/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C9A3BA-7BC2-5347-AB79-39313DF2D544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE36DDD2-DE13-AA44-96A3-27A14B840283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="3260" windowWidth="47240" windowHeight="22400" xr2:uid="{E56130A1-82B1-034C-9FBF-E21DD198A6C4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="1466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="1465">
   <si>
     <t>ACTACAGGCACTCTCCCTGGCTAGAAGGGCAGGATAATAACAAACAAGAGATKATTTAAAGCCAGAGAAGTGATGGGGG</t>
   </si>
@@ -3236,21 +3236,6 @@
     <t>SNPLocationsInReferenceSequence</t>
   </si>
   <si>
-    <t>AllSNPsRound1: 151, 158, 201; 8Amplicons22variants: 151, 158, 201, 209</t>
-  </si>
-  <si>
-    <t>AllSNPsRound1: 118, 151, 186; 8Amplicons22variants: 118, 151</t>
-  </si>
-  <si>
-    <t>AllSNPsRound1: 94, 151, 231; 24Amplicons53Variants: 151</t>
-  </si>
-  <si>
-    <t>AllSNPsRound1: 96, 130, 133, 151; 24Amplicons53Variants: 130, 133, 151</t>
-  </si>
-  <si>
-    <t>AllSNPsRound1: 151, 165, 172, 201; 24Amplicons53Variants: 151, 165, 172</t>
-  </si>
-  <si>
     <t>AmpliconGenomveV2Location</t>
   </si>
   <si>
@@ -4437,6 +4422,18 @@
   </si>
   <si>
     <t>129, 151</t>
+  </si>
+  <si>
+    <t>118, 151</t>
+  </si>
+  <si>
+    <t>151, 158, 201, 209</t>
+  </si>
+  <si>
+    <t>130, 133, 151</t>
+  </si>
+  <si>
+    <t>151, 165, 172</t>
   </si>
 </sst>
 </file>
@@ -4905,7 +4902,7 @@
   <dimension ref="A1:T205"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D189" workbookViewId="0">
-      <selection activeCell="H198" sqref="H198"/>
+      <selection activeCell="H206" sqref="H206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4930,7 +4927,7 @@
         <v>939</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1070</v>
+        <v>1065</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>526</v>
@@ -4951,7 +4948,7 @@
         <v>940</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>1071</v>
+        <v>1066</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>303</v>
@@ -4965,7 +4962,7 @@
         <v>312</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>1072</v>
+        <v>1067</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>559</v>
@@ -4986,7 +4983,7 @@
         <v>334</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -4997,7 +4994,7 @@
         <v>353</v>
       </c>
       <c r="C3" t="s">
-        <v>1073</v>
+        <v>1068</v>
       </c>
       <c r="D3" t="s">
         <v>764</v>
@@ -5012,7 +5009,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>1298</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -5023,7 +5020,7 @@
         <v>354</v>
       </c>
       <c r="C4" t="s">
-        <v>1074</v>
+        <v>1069</v>
       </c>
       <c r="D4" t="s">
         <v>757</v>
@@ -5038,7 +5035,7 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>1299</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -5049,7 +5046,7 @@
         <v>355</v>
       </c>
       <c r="C5" t="s">
-        <v>1075</v>
+        <v>1070</v>
       </c>
       <c r="D5" t="s">
         <v>557</v>
@@ -5075,7 +5072,7 @@
         <v>356</v>
       </c>
       <c r="C6" t="s">
-        <v>1076</v>
+        <v>1071</v>
       </c>
       <c r="D6" t="s">
         <v>930</v>
@@ -5090,7 +5087,7 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>1300</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -5101,7 +5098,7 @@
         <v>357</v>
       </c>
       <c r="C7" t="s">
-        <v>1077</v>
+        <v>1072</v>
       </c>
       <c r="D7" t="s">
         <v>750</v>
@@ -5127,7 +5124,7 @@
         <v>358</v>
       </c>
       <c r="C8" t="s">
-        <v>1078</v>
+        <v>1073</v>
       </c>
       <c r="D8" t="s">
         <v>747</v>
@@ -5142,7 +5139,7 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>1301</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -5153,7 +5150,7 @@
         <v>359</v>
       </c>
       <c r="C9" t="s">
-        <v>1079</v>
+        <v>1074</v>
       </c>
       <c r="D9" t="s">
         <v>745</v>
@@ -5168,7 +5165,7 @@
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>1302</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -5179,7 +5176,7 @@
         <v>360</v>
       </c>
       <c r="C10" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="D10" t="s">
         <v>622</v>
@@ -5194,7 +5191,7 @@
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>1303</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -5205,7 +5202,7 @@
         <v>361</v>
       </c>
       <c r="C11" t="s">
-        <v>1081</v>
+        <v>1076</v>
       </c>
       <c r="D11" t="s">
         <v>759</v>
@@ -5220,7 +5217,7 @@
         <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>1304</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -5231,7 +5228,7 @@
         <v>362</v>
       </c>
       <c r="C12" t="s">
-        <v>1082</v>
+        <v>1077</v>
       </c>
       <c r="D12" t="s">
         <v>620</v>
@@ -5246,7 +5243,7 @@
         <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>1305</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -5257,7 +5254,7 @@
         <v>363</v>
       </c>
       <c r="C13" t="s">
-        <v>1083</v>
+        <v>1078</v>
       </c>
       <c r="D13" t="s">
         <v>754</v>
@@ -5272,7 +5269,7 @@
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>1306</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -5283,7 +5280,7 @@
         <v>364</v>
       </c>
       <c r="C14" t="s">
-        <v>1084</v>
+        <v>1079</v>
       </c>
       <c r="D14" t="s">
         <v>618</v>
@@ -5309,7 +5306,7 @@
         <v>365</v>
       </c>
       <c r="C15" t="s">
-        <v>1085</v>
+        <v>1080</v>
       </c>
       <c r="D15" t="s">
         <v>616</v>
@@ -5324,7 +5321,7 @@
         <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>1307</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -5335,7 +5332,7 @@
         <v>366</v>
       </c>
       <c r="C16" t="s">
-        <v>1086</v>
+        <v>1081</v>
       </c>
       <c r="D16" t="s">
         <v>744</v>
@@ -5350,7 +5347,7 @@
         <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>1308</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -5361,7 +5358,7 @@
         <v>367</v>
       </c>
       <c r="C17" t="s">
-        <v>1087</v>
+        <v>1082</v>
       </c>
       <c r="D17" t="s">
         <v>633</v>
@@ -5376,7 +5373,7 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>1309</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -5387,7 +5384,7 @@
         <v>368</v>
       </c>
       <c r="C18" t="s">
-        <v>1088</v>
+        <v>1083</v>
       </c>
       <c r="D18" t="s">
         <v>614</v>
@@ -5413,7 +5410,7 @@
         <v>369</v>
       </c>
       <c r="C19" t="s">
-        <v>1089</v>
+        <v>1084</v>
       </c>
       <c r="D19" t="s">
         <v>612</v>
@@ -5428,7 +5425,7 @@
         <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>1310</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5439,7 +5436,7 @@
         <v>305</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>1090</v>
+        <v>1085</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>610</v>
@@ -5460,7 +5457,7 @@
         <v>330</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -5471,7 +5468,7 @@
         <v>370</v>
       </c>
       <c r="C21" t="s">
-        <v>1091</v>
+        <v>1086</v>
       </c>
       <c r="D21" t="s">
         <v>753</v>
@@ -5486,7 +5483,7 @@
         <v>19</v>
       </c>
       <c r="H21" t="s">
-        <v>1311</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -5497,7 +5494,7 @@
         <v>371</v>
       </c>
       <c r="C22" t="s">
-        <v>1092</v>
+        <v>1087</v>
       </c>
       <c r="D22" t="s">
         <v>608</v>
@@ -5512,7 +5509,7 @@
         <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>1312</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -5523,7 +5520,7 @@
         <v>372</v>
       </c>
       <c r="C23" t="s">
-        <v>1093</v>
+        <v>1088</v>
       </c>
       <c r="D23" t="s">
         <v>606</v>
@@ -5549,7 +5546,7 @@
         <v>373</v>
       </c>
       <c r="C24" t="s">
-        <v>1094</v>
+        <v>1089</v>
       </c>
       <c r="D24" t="s">
         <v>604</v>
@@ -5575,7 +5572,7 @@
         <v>374</v>
       </c>
       <c r="C25" t="s">
-        <v>1095</v>
+        <v>1090</v>
       </c>
       <c r="D25" t="s">
         <v>763</v>
@@ -5590,7 +5587,7 @@
         <v>23</v>
       </c>
       <c r="H25" t="s">
-        <v>1313</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -5601,7 +5598,7 @@
         <v>375</v>
       </c>
       <c r="C26" t="s">
-        <v>1096</v>
+        <v>1091</v>
       </c>
       <c r="D26" t="s">
         <v>602</v>
@@ -5616,7 +5613,7 @@
         <v>24</v>
       </c>
       <c r="H26" t="s">
-        <v>1314</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -5627,7 +5624,7 @@
         <v>376</v>
       </c>
       <c r="C27" t="s">
-        <v>1097</v>
+        <v>1092</v>
       </c>
       <c r="D27" t="s">
         <v>601</v>
@@ -5642,7 +5639,7 @@
         <v>25</v>
       </c>
       <c r="H27" t="s">
-        <v>1315</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5653,7 +5650,7 @@
         <v>306</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>1098</v>
+        <v>1093</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>599</v>
@@ -5668,13 +5665,13 @@
         <v>26</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>1316</v>
+        <v>1311</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>348</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -5685,7 +5682,7 @@
         <v>377</v>
       </c>
       <c r="C29" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
       <c r="D29" t="s">
         <v>749</v>
@@ -5700,7 +5697,7 @@
         <v>27</v>
       </c>
       <c r="H29" t="s">
-        <v>1317</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -5711,7 +5708,7 @@
         <v>378</v>
       </c>
       <c r="C30" t="s">
-        <v>1100</v>
+        <v>1095</v>
       </c>
       <c r="D30" t="s">
         <v>746</v>
@@ -5726,7 +5723,7 @@
         <v>28</v>
       </c>
       <c r="H30" t="s">
-        <v>1318</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -5737,7 +5734,7 @@
         <v>379</v>
       </c>
       <c r="C31" t="s">
-        <v>1101</v>
+        <v>1096</v>
       </c>
       <c r="D31" t="s">
         <v>597</v>
@@ -5763,7 +5760,7 @@
         <v>307</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>1102</v>
+        <v>1097</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>932</v>
@@ -5784,7 +5781,7 @@
         <v>331</v>
       </c>
       <c r="K32" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5795,7 +5792,7 @@
         <v>304</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>1103</v>
+        <v>1098</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>647</v>
@@ -5810,13 +5807,13 @@
         <v>31</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>1319</v>
+        <v>1314</v>
       </c>
       <c r="I33" s="13" t="s">
         <v>329</v>
       </c>
       <c r="K33" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -5827,7 +5824,7 @@
         <v>380</v>
       </c>
       <c r="C34" t="s">
-        <v>1104</v>
+        <v>1099</v>
       </c>
       <c r="D34" t="s">
         <v>595</v>
@@ -5853,7 +5850,7 @@
         <v>381</v>
       </c>
       <c r="C35" t="s">
-        <v>1105</v>
+        <v>1100</v>
       </c>
       <c r="D35" t="s">
         <v>641</v>
@@ -5868,7 +5865,7 @@
         <v>33</v>
       </c>
       <c r="H35" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -5879,7 +5876,7 @@
         <v>382</v>
       </c>
       <c r="C36" t="s">
-        <v>1106</v>
+        <v>1101</v>
       </c>
       <c r="D36" t="s">
         <v>593</v>
@@ -5905,7 +5902,7 @@
         <v>383</v>
       </c>
       <c r="C37" t="s">
-        <v>1107</v>
+        <v>1102</v>
       </c>
       <c r="D37" t="s">
         <v>639</v>
@@ -5920,7 +5917,7 @@
         <v>35</v>
       </c>
       <c r="H37" t="s">
-        <v>1321</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5931,7 +5928,7 @@
         <v>308</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>1108</v>
+        <v>1103</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>762</v>
@@ -5946,13 +5943,13 @@
         <v>36</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>1322</v>
+        <v>1317</v>
       </c>
       <c r="I38" s="13" t="s">
         <v>332</v>
       </c>
       <c r="K38" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -5963,7 +5960,7 @@
         <v>384</v>
       </c>
       <c r="C39" t="s">
-        <v>1109</v>
+        <v>1104</v>
       </c>
       <c r="D39" t="s">
         <v>649</v>
@@ -5978,7 +5975,7 @@
         <v>37</v>
       </c>
       <c r="H39" t="s">
-        <v>1323</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5989,7 +5986,7 @@
         <v>309</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1110</v>
+        <v>1105</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>756</v>
@@ -6004,16 +6001,16 @@
         <v>38</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>1324</v>
+        <v>1319</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>1284</v>
+        <v>1279</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>1277</v>
+        <v>1272</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>1296</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -6024,7 +6021,7 @@
         <v>385</v>
       </c>
       <c r="C41" t="s">
-        <v>1111</v>
+        <v>1106</v>
       </c>
       <c r="D41" t="s">
         <v>643</v>
@@ -6039,7 +6036,7 @@
         <v>39</v>
       </c>
       <c r="H41" t="s">
-        <v>1325</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -6050,7 +6047,7 @@
         <v>310</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>1112</v>
+        <v>1107</v>
       </c>
       <c r="D42" s="20" t="s">
         <v>591</v>
@@ -6071,10 +6068,10 @@
         <v>349</v>
       </c>
       <c r="J42" s="20" t="s">
-        <v>1276</v>
+        <v>1271</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>1282</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -6085,7 +6082,7 @@
         <v>386</v>
       </c>
       <c r="C43" t="s">
-        <v>1113</v>
+        <v>1108</v>
       </c>
       <c r="D43" t="s">
         <v>589</v>
@@ -6100,7 +6097,7 @@
         <v>41</v>
       </c>
       <c r="H43" t="s">
-        <v>1326</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -6111,7 +6108,7 @@
         <v>387</v>
       </c>
       <c r="C44" t="s">
-        <v>1114</v>
+        <v>1109</v>
       </c>
       <c r="D44" t="s">
         <v>587</v>
@@ -6126,7 +6123,7 @@
         <v>42</v>
       </c>
       <c r="H44" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -6137,7 +6134,7 @@
         <v>388</v>
       </c>
       <c r="C45" t="s">
-        <v>1115</v>
+        <v>1110</v>
       </c>
       <c r="D45" t="s">
         <v>761</v>
@@ -6152,7 +6149,7 @@
         <v>43</v>
       </c>
       <c r="H45" t="s">
-        <v>1327</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -6163,7 +6160,7 @@
         <v>389</v>
       </c>
       <c r="C46" t="s">
-        <v>1116</v>
+        <v>1111</v>
       </c>
       <c r="D46" t="s">
         <v>585</v>
@@ -6189,7 +6186,7 @@
         <v>390</v>
       </c>
       <c r="C47" t="s">
-        <v>1117</v>
+        <v>1112</v>
       </c>
       <c r="D47" t="s">
         <v>583</v>
@@ -6204,7 +6201,7 @@
         <v>45</v>
       </c>
       <c r="H47" t="s">
-        <v>1328</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -6215,7 +6212,7 @@
         <v>391</v>
       </c>
       <c r="C48" t="s">
-        <v>1118</v>
+        <v>1113</v>
       </c>
       <c r="D48" t="s">
         <v>755</v>
@@ -6241,7 +6238,7 @@
         <v>392</v>
       </c>
       <c r="C49" t="s">
-        <v>1119</v>
+        <v>1114</v>
       </c>
       <c r="D49" t="s">
         <v>579</v>
@@ -6267,7 +6264,7 @@
         <v>311</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>1120</v>
+        <v>1115</v>
       </c>
       <c r="D50" s="13" t="s">
         <v>577</v>
@@ -6282,13 +6279,13 @@
         <v>48</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>1329</v>
+        <v>1324</v>
       </c>
       <c r="I50" s="13" t="s">
         <v>333</v>
       </c>
       <c r="K50" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -6299,7 +6296,7 @@
         <v>393</v>
       </c>
       <c r="C51" t="s">
-        <v>1121</v>
+        <v>1116</v>
       </c>
       <c r="D51" t="s">
         <v>575</v>
@@ -6314,7 +6311,7 @@
         <v>49</v>
       </c>
       <c r="H51" t="s">
-        <v>1330</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -6325,7 +6322,7 @@
         <v>394</v>
       </c>
       <c r="C52" t="s">
-        <v>1122</v>
+        <v>1117</v>
       </c>
       <c r="D52" t="s">
         <v>637</v>
@@ -6340,7 +6337,7 @@
         <v>50</v>
       </c>
       <c r="H52" t="s">
-        <v>1331</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -6351,7 +6348,7 @@
         <v>395</v>
       </c>
       <c r="C53" t="s">
-        <v>1123</v>
+        <v>1118</v>
       </c>
       <c r="D53" t="s">
         <v>573</v>
@@ -6366,7 +6363,7 @@
         <v>51</v>
       </c>
       <c r="H53" t="s">
-        <v>1332</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -6377,7 +6374,7 @@
         <v>396</v>
       </c>
       <c r="C54" t="s">
-        <v>1124</v>
+        <v>1119</v>
       </c>
       <c r="D54" t="s">
         <v>571</v>
@@ -6392,7 +6389,7 @@
         <v>52</v>
       </c>
       <c r="H54" t="s">
-        <v>1333</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -6403,7 +6400,7 @@
         <v>397</v>
       </c>
       <c r="C55" t="s">
-        <v>1125</v>
+        <v>1120</v>
       </c>
       <c r="D55" t="s">
         <v>569</v>
@@ -6418,7 +6415,7 @@
         <v>53</v>
       </c>
       <c r="H55" t="s">
-        <v>1334</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -6429,7 +6426,7 @@
         <v>398</v>
       </c>
       <c r="C56" t="s">
-        <v>1126</v>
+        <v>1121</v>
       </c>
       <c r="D56" t="s">
         <v>567</v>
@@ -6455,7 +6452,7 @@
         <v>399</v>
       </c>
       <c r="C57" t="s">
-        <v>1127</v>
+        <v>1122</v>
       </c>
       <c r="D57" t="s">
         <v>565</v>
@@ -6470,7 +6467,7 @@
         <v>55</v>
       </c>
       <c r="H57" t="s">
-        <v>1335</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -6481,7 +6478,7 @@
         <v>400</v>
       </c>
       <c r="C58" t="s">
-        <v>1128</v>
+        <v>1123</v>
       </c>
       <c r="D58" t="s">
         <v>563</v>
@@ -6507,7 +6504,7 @@
         <v>401</v>
       </c>
       <c r="C59" t="s">
-        <v>1129</v>
+        <v>1124</v>
       </c>
       <c r="D59" t="s">
         <v>561</v>
@@ -6522,7 +6519,7 @@
         <v>57</v>
       </c>
       <c r="H59" t="s">
-        <v>1336</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -6533,7 +6530,7 @@
         <v>402</v>
       </c>
       <c r="C60" t="s">
-        <v>1130</v>
+        <v>1125</v>
       </c>
       <c r="D60" t="s">
         <v>743</v>
@@ -6548,7 +6545,7 @@
         <v>58</v>
       </c>
       <c r="H60" t="s">
-        <v>1337</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -6559,7 +6556,7 @@
         <v>403</v>
       </c>
       <c r="C61" t="s">
-        <v>1131</v>
+        <v>1126</v>
       </c>
       <c r="D61" t="s">
         <v>626</v>
@@ -6574,7 +6571,7 @@
         <v>59</v>
       </c>
       <c r="H61" t="s">
-        <v>1338</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -6585,7 +6582,7 @@
         <v>404</v>
       </c>
       <c r="C62" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="D62" t="s">
         <v>624</v>
@@ -6600,7 +6597,7 @@
         <v>60</v>
       </c>
       <c r="H62" t="s">
-        <v>1339</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -6611,7 +6608,7 @@
         <v>405</v>
       </c>
       <c r="C63" t="s">
-        <v>1133</v>
+        <v>1128</v>
       </c>
       <c r="D63" t="s">
         <v>748</v>
@@ -6626,7 +6623,7 @@
         <v>61</v>
       </c>
       <c r="H63" t="s">
-        <v>1340</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -6637,7 +6634,7 @@
         <v>406</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>1134</v>
+        <v>1129</v>
       </c>
       <c r="D64" s="11" t="s">
         <v>760</v>
@@ -6652,13 +6649,13 @@
         <v>62</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>1341</v>
+        <v>1336</v>
       </c>
       <c r="J64" s="11" t="s">
-        <v>1278</v>
+        <v>1273</v>
       </c>
       <c r="K64" s="12" t="s">
-        <v>1285</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -6669,7 +6666,7 @@
         <v>407</v>
       </c>
       <c r="C65" t="s">
-        <v>1135</v>
+        <v>1130</v>
       </c>
       <c r="D65" t="s">
         <v>758</v>
@@ -6695,7 +6692,7 @@
         <v>408</v>
       </c>
       <c r="C66" t="s">
-        <v>1136</v>
+        <v>1131</v>
       </c>
       <c r="D66" t="s">
         <v>645</v>
@@ -6710,7 +6707,7 @@
         <v>64</v>
       </c>
       <c r="H66" t="s">
-        <v>1342</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -6721,7 +6718,7 @@
         <v>409</v>
       </c>
       <c r="C67" t="s">
-        <v>1137</v>
+        <v>1132</v>
       </c>
       <c r="D67" t="s">
         <v>555</v>
@@ -6747,7 +6744,7 @@
         <v>410</v>
       </c>
       <c r="C68" t="s">
-        <v>1138</v>
+        <v>1133</v>
       </c>
       <c r="D68" t="s">
         <v>752</v>
@@ -6773,7 +6770,7 @@
         <v>411</v>
       </c>
       <c r="C69" t="s">
-        <v>1139</v>
+        <v>1134</v>
       </c>
       <c r="D69" t="s">
         <v>553</v>
@@ -6788,7 +6785,7 @@
         <v>67</v>
       </c>
       <c r="H69" t="s">
-        <v>1343</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -6799,7 +6796,7 @@
         <v>412</v>
       </c>
       <c r="C70" t="s">
-        <v>1140</v>
+        <v>1135</v>
       </c>
       <c r="D70" t="s">
         <v>931</v>
@@ -6825,7 +6822,7 @@
         <v>413</v>
       </c>
       <c r="C71" t="s">
-        <v>1141</v>
+        <v>1136</v>
       </c>
       <c r="D71" t="s">
         <v>551</v>
@@ -6840,7 +6837,7 @@
         <v>69</v>
       </c>
       <c r="H71" t="s">
-        <v>1344</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
@@ -6851,7 +6848,7 @@
         <v>414</v>
       </c>
       <c r="C72" t="s">
-        <v>1142</v>
+        <v>1137</v>
       </c>
       <c r="D72" t="s">
         <v>751</v>
@@ -6866,7 +6863,7 @@
         <v>70</v>
       </c>
       <c r="H72" t="s">
-        <v>1345</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="73" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -6877,7 +6874,7 @@
         <v>313</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>1143</v>
+        <v>1138</v>
       </c>
       <c r="D73" s="13" t="s">
         <v>549</v>
@@ -6892,13 +6889,13 @@
         <v>71</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>1346</v>
+        <v>1341</v>
       </c>
       <c r="I73" s="13" t="s">
         <v>335</v>
       </c>
       <c r="K73" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -6909,7 +6906,7 @@
         <v>415</v>
       </c>
       <c r="C74" t="s">
-        <v>1144</v>
+        <v>1139</v>
       </c>
       <c r="D74" t="s">
         <v>635</v>
@@ -6924,7 +6921,7 @@
         <v>72</v>
       </c>
       <c r="H74" t="s">
-        <v>1347</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -6935,7 +6932,7 @@
         <v>416</v>
       </c>
       <c r="C75" t="s">
-        <v>1145</v>
+        <v>1140</v>
       </c>
       <c r="D75" t="s">
         <v>543</v>
@@ -6950,7 +6947,7 @@
         <v>73</v>
       </c>
       <c r="H75" t="s">
-        <v>1348</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -6961,7 +6958,7 @@
         <v>417</v>
       </c>
       <c r="C76" t="s">
-        <v>1146</v>
+        <v>1141</v>
       </c>
       <c r="D76" t="s">
         <v>541</v>
@@ -6987,7 +6984,7 @@
         <v>418</v>
       </c>
       <c r="C77" t="s">
-        <v>1147</v>
+        <v>1142</v>
       </c>
       <c r="D77" t="s">
         <v>539</v>
@@ -7013,7 +7010,7 @@
         <v>419</v>
       </c>
       <c r="C78" t="s">
-        <v>1148</v>
+        <v>1143</v>
       </c>
       <c r="D78" t="s">
         <v>535</v>
@@ -7028,7 +7025,7 @@
         <v>76</v>
       </c>
       <c r="H78" t="s">
-        <v>1349</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -7039,7 +7036,7 @@
         <v>420</v>
       </c>
       <c r="C79" t="s">
-        <v>1149</v>
+        <v>1144</v>
       </c>
       <c r="D79" t="s">
         <v>667</v>
@@ -7065,7 +7062,7 @@
         <v>421</v>
       </c>
       <c r="C80" t="s">
-        <v>1150</v>
+        <v>1145</v>
       </c>
       <c r="D80" t="s">
         <v>533</v>
@@ -7091,7 +7088,7 @@
         <v>422</v>
       </c>
       <c r="C81" t="s">
-        <v>1151</v>
+        <v>1146</v>
       </c>
       <c r="D81" t="s">
         <v>677</v>
@@ -7106,7 +7103,7 @@
         <v>941</v>
       </c>
       <c r="H81" t="s">
-        <v>1350</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.2">
@@ -7117,7 +7114,7 @@
         <v>423</v>
       </c>
       <c r="C82" t="s">
-        <v>1152</v>
+        <v>1147</v>
       </c>
       <c r="D82" t="s">
         <v>771</v>
@@ -7132,7 +7129,7 @@
         <v>942</v>
       </c>
       <c r="H82" t="s">
-        <v>1351</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
@@ -7143,7 +7140,7 @@
         <v>424</v>
       </c>
       <c r="C83" t="s">
-        <v>1153</v>
+        <v>1148</v>
       </c>
       <c r="D83" t="s">
         <v>654</v>
@@ -7158,7 +7155,7 @@
         <v>943</v>
       </c>
       <c r="H83" t="s">
-        <v>1352</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="84" spans="1:20" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -7169,7 +7166,7 @@
         <v>529</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>1154</v>
+        <v>1149</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>807</v>
@@ -7184,10 +7181,10 @@
         <v>944</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>1353</v>
+        <v>1348</v>
       </c>
       <c r="K84" s="8" t="s">
-        <v>1280</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="85" spans="1:20" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -7198,7 +7195,7 @@
         <v>425</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>1155</v>
+        <v>1150</v>
       </c>
       <c r="D85" s="11" t="s">
         <v>713</v>
@@ -7213,13 +7210,13 @@
         <v>945</v>
       </c>
       <c r="H85" s="11" t="s">
-        <v>1354</v>
+        <v>1349</v>
       </c>
       <c r="J85" s="11" t="s">
-        <v>1279</v>
+        <v>1274</v>
       </c>
       <c r="K85" s="12" t="s">
-        <v>1285</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.2">
@@ -7230,7 +7227,7 @@
         <v>426</v>
       </c>
       <c r="C86" t="s">
-        <v>1156</v>
+        <v>1151</v>
       </c>
       <c r="D86" t="s">
         <v>691</v>
@@ -7245,7 +7242,7 @@
         <v>946</v>
       </c>
       <c r="H86" t="s">
-        <v>1355</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.2">
@@ -7256,7 +7253,7 @@
         <v>427</v>
       </c>
       <c r="C87" t="s">
-        <v>1157</v>
+        <v>1152</v>
       </c>
       <c r="D87" t="s">
         <v>837</v>
@@ -7271,7 +7268,7 @@
         <v>947</v>
       </c>
       <c r="H87" t="s">
-        <v>1356</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.2">
@@ -7282,7 +7279,7 @@
         <v>428</v>
       </c>
       <c r="C88" t="s">
-        <v>1158</v>
+        <v>1153</v>
       </c>
       <c r="D88" t="s">
         <v>836</v>
@@ -7297,7 +7294,7 @@
         <v>948</v>
       </c>
       <c r="H88" t="s">
-        <v>1357</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.2">
@@ -7308,7 +7305,7 @@
         <v>429</v>
       </c>
       <c r="C89" t="s">
-        <v>1159</v>
+        <v>1154</v>
       </c>
       <c r="D89" t="s">
         <v>806</v>
@@ -7323,7 +7320,7 @@
         <v>949</v>
       </c>
       <c r="H89" t="s">
-        <v>1358</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.2">
@@ -7334,7 +7331,7 @@
         <v>430</v>
       </c>
       <c r="C90" t="s">
-        <v>1160</v>
+        <v>1155</v>
       </c>
       <c r="D90" t="s">
         <v>815</v>
@@ -7349,7 +7346,7 @@
         <v>950</v>
       </c>
       <c r="H90" t="s">
-        <v>1359</v>
+        <v>1354</v>
       </c>
       <c r="N90" s="1"/>
     </row>
@@ -7361,7 +7358,7 @@
         <v>314</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>1161</v>
+        <v>1156</v>
       </c>
       <c r="D91" s="13" t="s">
         <v>805</v>
@@ -7376,13 +7373,13 @@
         <v>951</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>1360</v>
+        <v>1355</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>336</v>
       </c>
       <c r="K91" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
       <c r="N91" s="15"/>
       <c r="O91" s="15"/>
@@ -7400,7 +7397,7 @@
         <v>431</v>
       </c>
       <c r="C92" t="s">
-        <v>1162</v>
+        <v>1157</v>
       </c>
       <c r="D92" t="s">
         <v>769</v>
@@ -7415,7 +7412,7 @@
         <v>952</v>
       </c>
       <c r="H92" t="s">
-        <v>1361</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.2">
@@ -7426,7 +7423,7 @@
         <v>432</v>
       </c>
       <c r="C93" t="s">
-        <v>1163</v>
+        <v>1158</v>
       </c>
       <c r="D93" t="s">
         <v>767</v>
@@ -7441,7 +7438,7 @@
         <v>953</v>
       </c>
       <c r="H93" t="s">
-        <v>1362</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.2">
@@ -7452,7 +7449,7 @@
         <v>433</v>
       </c>
       <c r="C94" t="s">
-        <v>1164</v>
+        <v>1159</v>
       </c>
       <c r="D94" t="s">
         <v>711</v>
@@ -7467,7 +7464,7 @@
         <v>954</v>
       </c>
       <c r="H94" t="s">
-        <v>1363</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
@@ -7478,7 +7475,7 @@
         <v>434</v>
       </c>
       <c r="C95" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="D95" t="s">
         <v>905</v>
@@ -7493,7 +7490,7 @@
         <v>955</v>
       </c>
       <c r="H95" t="s">
-        <v>1364</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="96" spans="1:20" s="16" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -7504,7 +7501,7 @@
         <v>315</v>
       </c>
       <c r="C96" s="16" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="D96" s="16" t="s">
         <v>709</v>
@@ -7519,16 +7516,16 @@
         <v>956</v>
       </c>
       <c r="H96" s="16" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
       <c r="I96" s="16" t="s">
         <v>337</v>
       </c>
       <c r="J96" s="16" t="s">
-        <v>1291</v>
+        <v>1286</v>
       </c>
       <c r="K96" s="17" t="s">
-        <v>1295</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
@@ -7539,7 +7536,7 @@
         <v>435</v>
       </c>
       <c r="C97" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="D97" t="s">
         <v>904</v>
@@ -7554,7 +7551,7 @@
         <v>957</v>
       </c>
       <c r="H97" t="s">
-        <v>1366</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="98" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -7565,7 +7562,7 @@
         <v>316</v>
       </c>
       <c r="C98" s="13" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
       <c r="D98" s="13" t="s">
         <v>903</v>
@@ -7580,13 +7577,13 @@
         <v>958</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>1367</v>
+        <v>1362</v>
       </c>
       <c r="I98" s="13" t="s">
         <v>338</v>
       </c>
       <c r="K98" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
@@ -7597,7 +7594,7 @@
         <v>436</v>
       </c>
       <c r="C99" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
       <c r="D99" t="s">
         <v>902</v>
@@ -7612,7 +7609,7 @@
         <v>959</v>
       </c>
       <c r="H99" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
@@ -7623,7 +7620,7 @@
         <v>437</v>
       </c>
       <c r="C100" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="D100" t="s">
         <v>865</v>
@@ -7638,7 +7635,7 @@
         <v>960</v>
       </c>
       <c r="H100" t="s">
-        <v>1369</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
@@ -7649,7 +7646,7 @@
         <v>438</v>
       </c>
       <c r="C101" t="s">
-        <v>1171</v>
+        <v>1166</v>
       </c>
       <c r="D101" t="s">
         <v>817</v>
@@ -7664,7 +7661,7 @@
         <v>961</v>
       </c>
       <c r="H101" t="s">
-        <v>1370</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
@@ -7675,7 +7672,7 @@
         <v>439</v>
       </c>
       <c r="C102" t="s">
-        <v>1172</v>
+        <v>1167</v>
       </c>
       <c r="D102" t="s">
         <v>864</v>
@@ -7690,7 +7687,7 @@
         <v>962</v>
       </c>
       <c r="H102" t="s">
-        <v>1371</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
@@ -7701,7 +7698,7 @@
         <v>440</v>
       </c>
       <c r="C103" t="s">
-        <v>1173</v>
+        <v>1168</v>
       </c>
       <c r="D103" t="s">
         <v>717</v>
@@ -7716,7 +7713,7 @@
         <v>963</v>
       </c>
       <c r="H103" t="s">
-        <v>1372</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="104" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -7727,7 +7724,7 @@
         <v>325</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>1174</v>
+        <v>1169</v>
       </c>
       <c r="D104" s="13" t="s">
         <v>918</v>
@@ -7742,13 +7739,13 @@
         <v>964</v>
       </c>
       <c r="H104" s="13" t="s">
-        <v>1373</v>
+        <v>1368</v>
       </c>
       <c r="I104" s="13" t="s">
         <v>351</v>
       </c>
       <c r="K104" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
@@ -7759,7 +7756,7 @@
         <v>441</v>
       </c>
       <c r="C105" t="s">
-        <v>1175</v>
+        <v>1170</v>
       </c>
       <c r="D105" t="s">
         <v>669</v>
@@ -7774,7 +7771,7 @@
         <v>965</v>
       </c>
       <c r="H105" t="s">
-        <v>1374</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
@@ -7785,7 +7782,7 @@
         <v>442</v>
       </c>
       <c r="C106" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="D106" t="s">
         <v>901</v>
@@ -7800,7 +7797,7 @@
         <v>966</v>
       </c>
       <c r="H106" t="s">
-        <v>1375</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
@@ -7811,7 +7808,7 @@
         <v>443</v>
       </c>
       <c r="C107" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
       <c r="D107" t="s">
         <v>900</v>
@@ -7826,7 +7823,7 @@
         <v>967</v>
       </c>
       <c r="H107" t="s">
-        <v>1376</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
@@ -7837,7 +7834,7 @@
         <v>444</v>
       </c>
       <c r="C108" t="s">
-        <v>1178</v>
+        <v>1173</v>
       </c>
       <c r="D108" t="s">
         <v>811</v>
@@ -7852,7 +7849,7 @@
         <v>968</v>
       </c>
       <c r="H108" t="s">
-        <v>1377</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
@@ -7863,7 +7860,7 @@
         <v>445</v>
       </c>
       <c r="C109" t="s">
-        <v>1179</v>
+        <v>1174</v>
       </c>
       <c r="D109" t="s">
         <v>631</v>
@@ -7878,7 +7875,7 @@
         <v>969</v>
       </c>
       <c r="H109" t="s">
-        <v>1378</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
@@ -7889,7 +7886,7 @@
         <v>446</v>
       </c>
       <c r="C110" t="s">
-        <v>1180</v>
+        <v>1175</v>
       </c>
       <c r="D110" t="s">
         <v>899</v>
@@ -7904,7 +7901,7 @@
         <v>970</v>
       </c>
       <c r="H110" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
@@ -7915,7 +7912,7 @@
         <v>447</v>
       </c>
       <c r="C111" t="s">
-        <v>1181</v>
+        <v>1176</v>
       </c>
       <c r="D111" t="s">
         <v>898</v>
@@ -7930,7 +7927,7 @@
         <v>971</v>
       </c>
       <c r="H111" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
@@ -7941,7 +7938,7 @@
         <v>448</v>
       </c>
       <c r="C112" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="D112" t="s">
         <v>804</v>
@@ -7956,7 +7953,7 @@
         <v>972</v>
       </c>
       <c r="H112" t="s">
-        <v>1381</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="113" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -7967,7 +7964,7 @@
         <v>317</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>1183</v>
+        <v>1178</v>
       </c>
       <c r="D113" s="13" t="s">
         <v>693</v>
@@ -7982,13 +7979,13 @@
         <v>973</v>
       </c>
       <c r="H113" s="13" t="s">
-        <v>1382</v>
+        <v>1377</v>
       </c>
       <c r="I113" s="13" t="s">
         <v>339</v>
       </c>
       <c r="K113" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
@@ -7999,7 +7996,7 @@
         <v>449</v>
       </c>
       <c r="C114" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="D114" t="s">
         <v>803</v>
@@ -8014,7 +8011,7 @@
         <v>974</v>
       </c>
       <c r="H114" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
@@ -8025,7 +8022,7 @@
         <v>450</v>
       </c>
       <c r="C115" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="D115" t="s">
         <v>897</v>
@@ -8040,7 +8037,7 @@
         <v>975</v>
       </c>
       <c r="H115" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="116" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -8051,7 +8048,7 @@
         <v>318</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>1186</v>
+        <v>1181</v>
       </c>
       <c r="D116" s="13" t="s">
         <v>664</v>
@@ -8066,13 +8063,13 @@
         <v>976</v>
       </c>
       <c r="H116" s="13" t="s">
-        <v>1385</v>
+        <v>1380</v>
       </c>
       <c r="I116" s="13" t="s">
         <v>340</v>
       </c>
       <c r="K116" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
@@ -8083,7 +8080,7 @@
         <v>451</v>
       </c>
       <c r="C117" t="s">
-        <v>1187</v>
+        <v>1182</v>
       </c>
       <c r="D117" t="s">
         <v>896</v>
@@ -8098,7 +8095,7 @@
         <v>977</v>
       </c>
       <c r="H117" t="s">
-        <v>1386</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
@@ -8109,7 +8106,7 @@
         <v>452</v>
       </c>
       <c r="C118" t="s">
-        <v>1188</v>
+        <v>1183</v>
       </c>
       <c r="D118" t="s">
         <v>885</v>
@@ -8124,7 +8121,7 @@
         <v>978</v>
       </c>
       <c r="H118" t="s">
-        <v>1387</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
@@ -8135,7 +8132,7 @@
         <v>453</v>
       </c>
       <c r="C119" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="D119" t="s">
         <v>835</v>
@@ -8150,7 +8147,7 @@
         <v>979</v>
       </c>
       <c r="H119" t="s">
-        <v>1388</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
@@ -8161,7 +8158,7 @@
         <v>454</v>
       </c>
       <c r="C120" t="s">
-        <v>1190</v>
+        <v>1185</v>
       </c>
       <c r="D120" t="s">
         <v>707</v>
@@ -8176,7 +8173,7 @@
         <v>980</v>
       </c>
       <c r="H120" t="s">
-        <v>1389</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
@@ -8187,7 +8184,7 @@
         <v>455</v>
       </c>
       <c r="C121" t="s">
-        <v>1191</v>
+        <v>1186</v>
       </c>
       <c r="D121" t="s">
         <v>884</v>
@@ -8202,7 +8199,7 @@
         <v>981</v>
       </c>
       <c r="H121" t="s">
-        <v>1390</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
@@ -8213,7 +8210,7 @@
         <v>456</v>
       </c>
       <c r="C122" t="s">
-        <v>1192</v>
+        <v>1187</v>
       </c>
       <c r="D122" t="s">
         <v>802</v>
@@ -8228,7 +8225,7 @@
         <v>982</v>
       </c>
       <c r="H122" t="s">
-        <v>1391</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
@@ -8239,7 +8236,7 @@
         <v>457</v>
       </c>
       <c r="C123" t="s">
-        <v>1193</v>
+        <v>1188</v>
       </c>
       <c r="D123" t="s">
         <v>823</v>
@@ -8254,7 +8251,7 @@
         <v>983</v>
       </c>
       <c r="H123" t="s">
-        <v>1392</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
@@ -8265,7 +8262,7 @@
         <v>458</v>
       </c>
       <c r="C124" t="s">
-        <v>1194</v>
+        <v>1189</v>
       </c>
       <c r="D124" t="s">
         <v>923</v>
@@ -8280,7 +8277,7 @@
         <v>984</v>
       </c>
       <c r="H124" t="s">
-        <v>1393</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="125" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -8291,7 +8288,7 @@
         <v>319</v>
       </c>
       <c r="C125" s="13" t="s">
-        <v>1195</v>
+        <v>1190</v>
       </c>
       <c r="D125" s="13" t="s">
         <v>687</v>
@@ -8306,13 +8303,13 @@
         <v>985</v>
       </c>
       <c r="H125" s="13" t="s">
-        <v>1394</v>
+        <v>1389</v>
       </c>
       <c r="I125" s="13" t="s">
         <v>341</v>
       </c>
       <c r="K125" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
@@ -8323,7 +8320,7 @@
         <v>459</v>
       </c>
       <c r="C126" t="s">
-        <v>1196</v>
+        <v>1191</v>
       </c>
       <c r="D126" t="s">
         <v>822</v>
@@ -8338,7 +8335,7 @@
         <v>986</v>
       </c>
       <c r="H126" t="s">
-        <v>1395</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
@@ -8349,7 +8346,7 @@
         <v>460</v>
       </c>
       <c r="C127" t="s">
-        <v>1197</v>
+        <v>1192</v>
       </c>
       <c r="D127" t="s">
         <v>675</v>
@@ -8364,7 +8361,7 @@
         <v>987</v>
       </c>
       <c r="H127" t="s">
-        <v>1396</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
@@ -8375,7 +8372,7 @@
         <v>461</v>
       </c>
       <c r="C128" t="s">
-        <v>1198</v>
+        <v>1193</v>
       </c>
       <c r="D128" t="s">
         <v>650</v>
@@ -8390,7 +8387,7 @@
         <v>988</v>
       </c>
       <c r="H128" t="s">
-        <v>1397</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.2">
@@ -8401,7 +8398,7 @@
         <v>462</v>
       </c>
       <c r="C129" t="s">
-        <v>1199</v>
+        <v>1194</v>
       </c>
       <c r="D129" t="s">
         <v>705</v>
@@ -8416,7 +8413,7 @@
         <v>989</v>
       </c>
       <c r="H129" t="s">
-        <v>1398</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
@@ -8427,7 +8424,7 @@
         <v>463</v>
       </c>
       <c r="C130" t="s">
-        <v>1200</v>
+        <v>1195</v>
       </c>
       <c r="D130" t="s">
         <v>922</v>
@@ -8442,7 +8439,7 @@
         <v>990</v>
       </c>
       <c r="H130" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.2">
@@ -8453,7 +8450,7 @@
         <v>464</v>
       </c>
       <c r="C131" t="s">
-        <v>1201</v>
+        <v>1196</v>
       </c>
       <c r="D131" t="s">
         <v>685</v>
@@ -8468,7 +8465,7 @@
         <v>991</v>
       </c>
       <c r="H131" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.2">
@@ -8479,7 +8476,7 @@
         <v>465</v>
       </c>
       <c r="C132" t="s">
-        <v>1202</v>
+        <v>1197</v>
       </c>
       <c r="D132" t="s">
         <v>810</v>
@@ -8494,7 +8491,7 @@
         <v>992</v>
       </c>
       <c r="H132" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="133" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -8505,7 +8502,7 @@
         <v>320</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>1203</v>
+        <v>1198</v>
       </c>
       <c r="D133" s="13" t="s">
         <v>703</v>
@@ -8520,13 +8517,13 @@
         <v>993</v>
       </c>
       <c r="H133" s="13" t="s">
-        <v>1402</v>
+        <v>1397</v>
       </c>
       <c r="I133" s="13" t="s">
         <v>342</v>
       </c>
       <c r="K133" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
@@ -8537,7 +8534,7 @@
         <v>466</v>
       </c>
       <c r="C134" t="s">
-        <v>1204</v>
+        <v>1199</v>
       </c>
       <c r="D134" t="s">
         <v>921</v>
@@ -8552,7 +8549,7 @@
         <v>994</v>
       </c>
       <c r="H134" t="s">
-        <v>1403</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
@@ -8563,7 +8560,7 @@
         <v>467</v>
       </c>
       <c r="C135" t="s">
-        <v>1205</v>
+        <v>1200</v>
       </c>
       <c r="D135" t="s">
         <v>883</v>
@@ -8578,7 +8575,7 @@
         <v>995</v>
       </c>
       <c r="H135" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
@@ -8589,7 +8586,7 @@
         <v>468</v>
       </c>
       <c r="C136" t="s">
-        <v>1206</v>
+        <v>1201</v>
       </c>
       <c r="D136" t="s">
         <v>701</v>
@@ -8604,7 +8601,7 @@
         <v>996</v>
       </c>
       <c r="H136" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.2">
@@ -8615,7 +8612,7 @@
         <v>469</v>
       </c>
       <c r="C137" t="s">
-        <v>1207</v>
+        <v>1202</v>
       </c>
       <c r="D137" t="s">
         <v>882</v>
@@ -8630,7 +8627,7 @@
         <v>997</v>
       </c>
       <c r="H137" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="138" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -8641,7 +8638,7 @@
         <v>321</v>
       </c>
       <c r="C138" s="13" t="s">
-        <v>1208</v>
+        <v>1203</v>
       </c>
       <c r="D138" s="13" t="s">
         <v>673</v>
@@ -8656,13 +8653,13 @@
         <v>998</v>
       </c>
       <c r="H138" s="13" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
       <c r="I138" s="13" t="s">
         <v>350</v>
       </c>
       <c r="K138" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="139" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -8673,7 +8670,7 @@
         <v>322</v>
       </c>
       <c r="C139" s="13" t="s">
-        <v>1209</v>
+        <v>1204</v>
       </c>
       <c r="D139" s="13" t="s">
         <v>881</v>
@@ -8688,13 +8685,13 @@
         <v>999</v>
       </c>
       <c r="H139" s="13" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
       <c r="I139" s="13" t="s">
         <v>343</v>
       </c>
       <c r="K139" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.2">
@@ -8705,7 +8702,7 @@
         <v>470</v>
       </c>
       <c r="C140" t="s">
-        <v>1210</v>
+        <v>1205</v>
       </c>
       <c r="D140" t="s">
         <v>880</v>
@@ -8720,7 +8717,7 @@
         <v>1000</v>
       </c>
       <c r="H140" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.2">
@@ -8731,7 +8728,7 @@
         <v>471</v>
       </c>
       <c r="C141" t="s">
-        <v>1211</v>
+        <v>1206</v>
       </c>
       <c r="D141" t="s">
         <v>671</v>
@@ -8746,7 +8743,7 @@
         <v>1001</v>
       </c>
       <c r="H141" t="s">
-        <v>1410</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.2">
@@ -8757,7 +8754,7 @@
         <v>472</v>
       </c>
       <c r="C142" t="s">
-        <v>1212</v>
+        <v>1207</v>
       </c>
       <c r="D142" t="s">
         <v>699</v>
@@ -8772,7 +8769,7 @@
         <v>1002</v>
       </c>
       <c r="H142" t="s">
-        <v>1411</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.2">
@@ -8783,7 +8780,7 @@
         <v>473</v>
       </c>
       <c r="C143" t="s">
-        <v>1213</v>
+        <v>1208</v>
       </c>
       <c r="D143" t="s">
         <v>920</v>
@@ -8798,7 +8795,7 @@
         <v>1003</v>
       </c>
       <c r="H143" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="144" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -8809,7 +8806,7 @@
         <v>323</v>
       </c>
       <c r="C144" s="13" t="s">
-        <v>1214</v>
+        <v>1209</v>
       </c>
       <c r="D144" s="13" t="s">
         <v>663</v>
@@ -8824,13 +8821,13 @@
         <v>1004</v>
       </c>
       <c r="H144" s="13" t="s">
-        <v>1413</v>
+        <v>1408</v>
       </c>
       <c r="I144" s="13" t="s">
         <v>344</v>
       </c>
       <c r="K144" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.2">
@@ -8841,7 +8838,7 @@
         <v>474</v>
       </c>
       <c r="C145" t="s">
-        <v>1215</v>
+        <v>1210</v>
       </c>
       <c r="D145" t="s">
         <v>919</v>
@@ -8856,7 +8853,7 @@
         <v>1005</v>
       </c>
       <c r="H145" t="s">
-        <v>1414</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.2">
@@ -8867,7 +8864,7 @@
         <v>475</v>
       </c>
       <c r="C146" t="s">
-        <v>1216</v>
+        <v>1211</v>
       </c>
       <c r="D146" t="s">
         <v>879</v>
@@ -8882,7 +8879,7 @@
         <v>1006</v>
       </c>
       <c r="H146" t="s">
-        <v>1415</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="147" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -8893,7 +8890,7 @@
         <v>324</v>
       </c>
       <c r="C147" s="13" t="s">
-        <v>1217</v>
+        <v>1212</v>
       </c>
       <c r="D147" s="13" t="s">
         <v>878</v>
@@ -8908,13 +8905,13 @@
         <v>1007</v>
       </c>
       <c r="H147" s="13" t="s">
-        <v>1416</v>
+        <v>1411</v>
       </c>
       <c r="I147" s="13" t="s">
         <v>345</v>
       </c>
       <c r="K147" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="148" spans="1:11" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -8925,7 +8922,7 @@
         <v>476</v>
       </c>
       <c r="C148" s="18" t="s">
-        <v>1218</v>
+        <v>1213</v>
       </c>
       <c r="D148" s="18" t="s">
         <v>877</v>
@@ -8940,10 +8937,10 @@
         <v>1008</v>
       </c>
       <c r="H148" s="18" t="s">
-        <v>1417</v>
+        <v>1412</v>
       </c>
       <c r="K148" s="19" t="s">
-        <v>1292</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.2">
@@ -8954,7 +8951,7 @@
         <v>477</v>
       </c>
       <c r="C149" t="s">
-        <v>1219</v>
+        <v>1214</v>
       </c>
       <c r="D149" t="s">
         <v>821</v>
@@ -8969,7 +8966,7 @@
         <v>1009</v>
       </c>
       <c r="H149" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.2">
@@ -8980,7 +8977,7 @@
         <v>478</v>
       </c>
       <c r="C150" t="s">
-        <v>1220</v>
+        <v>1215</v>
       </c>
       <c r="D150" t="s">
         <v>657</v>
@@ -8995,7 +8992,7 @@
         <v>1010</v>
       </c>
       <c r="H150" t="s">
-        <v>1419</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.2">
@@ -9006,7 +9003,7 @@
         <v>479</v>
       </c>
       <c r="C151" t="s">
-        <v>1221</v>
+        <v>1216</v>
       </c>
       <c r="D151" t="s">
         <v>697</v>
@@ -9021,7 +9018,7 @@
         <v>1011</v>
       </c>
       <c r="H151" t="s">
-        <v>1420</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.2">
@@ -9032,7 +9029,7 @@
         <v>480</v>
       </c>
       <c r="C152" t="s">
-        <v>1222</v>
+        <v>1217</v>
       </c>
       <c r="D152" t="s">
         <v>695</v>
@@ -9047,7 +9044,7 @@
         <v>1012</v>
       </c>
       <c r="H152" t="s">
-        <v>1421</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.2">
@@ -9058,7 +9055,7 @@
         <v>481</v>
       </c>
       <c r="C153" t="s">
-        <v>1223</v>
+        <v>1218</v>
       </c>
       <c r="D153" t="s">
         <v>876</v>
@@ -9073,7 +9070,7 @@
         <v>1013</v>
       </c>
       <c r="H153" t="s">
-        <v>1422</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="154" spans="1:11" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -9084,7 +9081,7 @@
         <v>530</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>1224</v>
+        <v>1219</v>
       </c>
       <c r="D154" s="7" t="s">
         <v>652</v>
@@ -9099,10 +9096,10 @@
         <v>1014</v>
       </c>
       <c r="H154" s="7" t="s">
-        <v>1423</v>
+        <v>1418</v>
       </c>
       <c r="K154" s="8" t="s">
-        <v>1281</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.2">
@@ -9113,7 +9110,7 @@
         <v>482</v>
       </c>
       <c r="C155" t="s">
-        <v>1225</v>
+        <v>1220</v>
       </c>
       <c r="D155" t="s">
         <v>809</v>
@@ -9128,7 +9125,7 @@
         <v>1015</v>
       </c>
       <c r="H155" t="s">
-        <v>1424</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.2">
@@ -9139,7 +9136,7 @@
         <v>483</v>
       </c>
       <c r="C156" t="s">
-        <v>1226</v>
+        <v>1221</v>
       </c>
       <c r="D156" t="s">
         <v>917</v>
@@ -9154,7 +9151,7 @@
         <v>1016</v>
       </c>
       <c r="H156" t="s">
-        <v>1425</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.2">
@@ -9165,7 +9162,7 @@
         <v>484</v>
       </c>
       <c r="C157" t="s">
-        <v>1227</v>
+        <v>1222</v>
       </c>
       <c r="D157" t="s">
         <v>715</v>
@@ -9180,7 +9177,7 @@
         <v>1017</v>
       </c>
       <c r="H157" t="s">
-        <v>1426</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="158" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -9191,7 +9188,7 @@
         <v>326</v>
       </c>
       <c r="C158" s="13" t="s">
-        <v>1228</v>
+        <v>1223</v>
       </c>
       <c r="D158" s="13" t="s">
         <v>683</v>
@@ -9206,13 +9203,13 @@
         <v>1018</v>
       </c>
       <c r="H158" s="13" t="s">
-        <v>1427</v>
+        <v>1422</v>
       </c>
       <c r="I158" s="13" t="s">
         <v>352</v>
       </c>
       <c r="K158" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.2">
@@ -9223,7 +9220,7 @@
         <v>485</v>
       </c>
       <c r="C159" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D159" t="s">
         <v>863</v>
@@ -9238,7 +9235,7 @@
         <v>1019</v>
       </c>
       <c r="H159" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.2">
@@ -9249,7 +9246,7 @@
         <v>486</v>
       </c>
       <c r="C160" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D160" t="s">
         <v>862</v>
@@ -9264,7 +9261,7 @@
         <v>1020</v>
       </c>
       <c r="H160" t="s">
-        <v>1429</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.2">
@@ -9275,7 +9272,7 @@
         <v>487</v>
       </c>
       <c r="C161" t="s">
-        <v>1231</v>
+        <v>1226</v>
       </c>
       <c r="D161" t="s">
         <v>916</v>
@@ -9290,7 +9287,7 @@
         <v>1021</v>
       </c>
       <c r="H161" t="s">
-        <v>1430</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.2">
@@ -9301,7 +9298,7 @@
         <v>488</v>
       </c>
       <c r="C162" t="s">
-        <v>1232</v>
+        <v>1227</v>
       </c>
       <c r="D162" t="s">
         <v>861</v>
@@ -9316,7 +9313,7 @@
         <v>1022</v>
       </c>
       <c r="H162" t="s">
-        <v>1431</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.2">
@@ -9327,7 +9324,7 @@
         <v>489</v>
       </c>
       <c r="C163" t="s">
-        <v>1233</v>
+        <v>1228</v>
       </c>
       <c r="D163" t="s">
         <v>860</v>
@@ -9342,7 +9339,7 @@
         <v>1023</v>
       </c>
       <c r="H163" t="s">
-        <v>1432</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="164" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -9353,7 +9350,7 @@
         <v>327</v>
       </c>
       <c r="C164" s="13" t="s">
-        <v>1234</v>
+        <v>1229</v>
       </c>
       <c r="D164" s="13" t="s">
         <v>859</v>
@@ -9368,13 +9365,13 @@
         <v>1024</v>
       </c>
       <c r="H164" s="13" t="s">
-        <v>1433</v>
+        <v>1428</v>
       </c>
       <c r="I164" s="13" t="s">
         <v>346</v>
       </c>
       <c r="K164" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.2">
@@ -9385,7 +9382,7 @@
         <v>490</v>
       </c>
       <c r="C165" t="s">
-        <v>1235</v>
+        <v>1230</v>
       </c>
       <c r="D165" t="s">
         <v>834</v>
@@ -9400,7 +9397,7 @@
         <v>1025</v>
       </c>
       <c r="H165" t="s">
-        <v>1434</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.2">
@@ -9411,7 +9408,7 @@
         <v>491</v>
       </c>
       <c r="C166" t="s">
-        <v>1236</v>
+        <v>1231</v>
       </c>
       <c r="D166" t="s">
         <v>858</v>
@@ -9426,7 +9423,7 @@
         <v>1026</v>
       </c>
       <c r="H166" t="s">
-        <v>1435</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.2">
@@ -9437,7 +9434,7 @@
         <v>492</v>
       </c>
       <c r="C167" t="s">
-        <v>1237</v>
+        <v>1232</v>
       </c>
       <c r="D167" t="s">
         <v>857</v>
@@ -9452,7 +9449,7 @@
         <v>1027</v>
       </c>
       <c r="H167" t="s">
-        <v>1436</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.2">
@@ -9463,7 +9460,7 @@
         <v>493</v>
       </c>
       <c r="C168" t="s">
-        <v>1238</v>
+        <v>1233</v>
       </c>
       <c r="D168" t="s">
         <v>689</v>
@@ -9478,7 +9475,7 @@
         <v>1028</v>
       </c>
       <c r="H168" t="s">
-        <v>1437</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.2">
@@ -9489,7 +9486,7 @@
         <v>494</v>
       </c>
       <c r="C169" t="s">
-        <v>1239</v>
+        <v>1234</v>
       </c>
       <c r="D169" t="s">
         <v>661</v>
@@ -9504,7 +9501,7 @@
         <v>1029</v>
       </c>
       <c r="H169" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.2">
@@ -9515,7 +9512,7 @@
         <v>495</v>
       </c>
       <c r="C170" t="s">
-        <v>1240</v>
+        <v>1235</v>
       </c>
       <c r="D170" t="s">
         <v>659</v>
@@ -9530,7 +9527,7 @@
         <v>1030</v>
       </c>
       <c r="H170" t="s">
-        <v>1439</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.2">
@@ -9541,7 +9538,7 @@
         <v>496</v>
       </c>
       <c r="C171" t="s">
-        <v>1241</v>
+        <v>1236</v>
       </c>
       <c r="D171" t="s">
         <v>856</v>
@@ -9556,7 +9553,7 @@
         <v>1031</v>
       </c>
       <c r="H171" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="172" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -9567,7 +9564,7 @@
         <v>328</v>
       </c>
       <c r="C172" s="13" t="s">
-        <v>1242</v>
+        <v>1237</v>
       </c>
       <c r="D172" s="13" t="s">
         <v>855</v>
@@ -9582,13 +9579,13 @@
         <v>1032</v>
       </c>
       <c r="H172" s="13" t="s">
-        <v>1441</v>
+        <v>1436</v>
       </c>
       <c r="I172" s="13" t="s">
         <v>347</v>
       </c>
       <c r="K172" s="14" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.2">
@@ -9599,7 +9596,7 @@
         <v>497</v>
       </c>
       <c r="C173" t="s">
-        <v>1243</v>
+        <v>1238</v>
       </c>
       <c r="D173" t="s">
         <v>843</v>
@@ -9614,7 +9611,7 @@
         <v>1033</v>
       </c>
       <c r="H173" t="s">
-        <v>1442</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.2">
@@ -9625,7 +9622,7 @@
         <v>498</v>
       </c>
       <c r="C174" t="s">
-        <v>1244</v>
+        <v>1239</v>
       </c>
       <c r="D174" t="s">
         <v>915</v>
@@ -9640,7 +9637,7 @@
         <v>1034</v>
       </c>
       <c r="H174" t="s">
-        <v>1443</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.2">
@@ -9651,7 +9648,7 @@
         <v>499</v>
       </c>
       <c r="C175" t="s">
-        <v>1245</v>
+        <v>1240</v>
       </c>
       <c r="D175" t="s">
         <v>773</v>
@@ -9666,7 +9663,7 @@
         <v>1035</v>
       </c>
       <c r="H175" t="s">
-        <v>1444</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.2">
@@ -9677,7 +9674,7 @@
         <v>500</v>
       </c>
       <c r="C176" t="s">
-        <v>1246</v>
+        <v>1241</v>
       </c>
       <c r="D176" t="s">
         <v>719</v>
@@ -9692,7 +9689,7 @@
         <v>1036</v>
       </c>
       <c r="H176" t="s">
-        <v>1445</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
@@ -9703,7 +9700,7 @@
         <v>501</v>
       </c>
       <c r="C177" t="s">
-        <v>1247</v>
+        <v>1242</v>
       </c>
       <c r="D177" t="s">
         <v>842</v>
@@ -9718,7 +9715,7 @@
         <v>1037</v>
       </c>
       <c r="H177" t="s">
-        <v>1446</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
@@ -9729,7 +9726,7 @@
         <v>502</v>
       </c>
       <c r="C178" t="s">
-        <v>1248</v>
+        <v>1243</v>
       </c>
       <c r="D178" t="s">
         <v>841</v>
@@ -9744,7 +9741,7 @@
         <v>1038</v>
       </c>
       <c r="H178" t="s">
-        <v>1447</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
@@ -9755,7 +9752,7 @@
         <v>503</v>
       </c>
       <c r="C179" t="s">
-        <v>1249</v>
+        <v>1244</v>
       </c>
       <c r="D179" t="s">
         <v>840</v>
@@ -9770,7 +9767,7 @@
         <v>1039</v>
       </c>
       <c r="H179" t="s">
-        <v>1448</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
@@ -9781,7 +9778,7 @@
         <v>504</v>
       </c>
       <c r="C180" t="s">
-        <v>1250</v>
+        <v>1245</v>
       </c>
       <c r="D180" t="s">
         <v>808</v>
@@ -9796,7 +9793,7 @@
         <v>1040</v>
       </c>
       <c r="H180" t="s">
-        <v>1449</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
@@ -9807,7 +9804,7 @@
         <v>505</v>
       </c>
       <c r="C181" t="s">
-        <v>1251</v>
+        <v>1246</v>
       </c>
       <c r="D181" t="s">
         <v>775</v>
@@ -9822,7 +9819,7 @@
         <v>1041</v>
       </c>
       <c r="H181" t="s">
-        <v>1450</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
@@ -9833,7 +9830,7 @@
         <v>506</v>
       </c>
       <c r="C182" t="s">
-        <v>1252</v>
+        <v>1247</v>
       </c>
       <c r="D182" t="s">
         <v>839</v>
@@ -9848,7 +9845,7 @@
         <v>1042</v>
       </c>
       <c r="H182" t="s">
-        <v>1451</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
@@ -9859,7 +9856,7 @@
         <v>507</v>
       </c>
       <c r="C183" t="s">
-        <v>1253</v>
+        <v>1248</v>
       </c>
       <c r="D183" t="s">
         <v>838</v>
@@ -9874,7 +9871,7 @@
         <v>1043</v>
       </c>
       <c r="H183" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
@@ -9885,7 +9882,7 @@
         <v>508</v>
       </c>
       <c r="C184" t="s">
-        <v>1254</v>
+        <v>1249</v>
       </c>
       <c r="D184" t="s">
         <v>816</v>
@@ -9900,7 +9897,7 @@
         <v>1044</v>
       </c>
       <c r="H184" t="s">
-        <v>1453</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
@@ -9911,7 +9908,7 @@
         <v>509</v>
       </c>
       <c r="C185" t="s">
-        <v>1255</v>
+        <v>1250</v>
       </c>
       <c r="D185" t="s">
         <v>681</v>
@@ -9926,7 +9923,7 @@
         <v>1045</v>
       </c>
       <c r="H185" t="s">
-        <v>1454</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
@@ -9937,7 +9934,7 @@
         <v>510</v>
       </c>
       <c r="C186" t="s">
-        <v>1256</v>
+        <v>1251</v>
       </c>
       <c r="D186" t="s">
         <v>679</v>
@@ -9952,7 +9949,7 @@
         <v>1046</v>
       </c>
       <c r="H186" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
@@ -9963,7 +9960,7 @@
         <v>511</v>
       </c>
       <c r="C187" t="s">
-        <v>1257</v>
+        <v>1252</v>
       </c>
       <c r="D187" t="s">
         <v>721</v>
@@ -9978,7 +9975,7 @@
         <v>79</v>
       </c>
       <c r="H187" t="s">
-        <v>1456</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
@@ -9989,7 +9986,7 @@
         <v>512</v>
       </c>
       <c r="C188" t="s">
-        <v>1258</v>
+        <v>1253</v>
       </c>
       <c r="D188" t="s">
         <v>785</v>
@@ -10004,7 +10001,7 @@
         <v>80</v>
       </c>
       <c r="H188" t="s">
-        <v>1457</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
@@ -10015,7 +10012,7 @@
         <v>513</v>
       </c>
       <c r="C189" t="s">
-        <v>1259</v>
+        <v>1254</v>
       </c>
       <c r="D189" t="s">
         <v>581</v>
@@ -10030,7 +10027,7 @@
         <v>81</v>
       </c>
       <c r="H189" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
@@ -10041,7 +10038,7 @@
         <v>514</v>
       </c>
       <c r="C190" t="s">
-        <v>1260</v>
+        <v>1255</v>
       </c>
       <c r="D190" t="s">
         <v>629</v>
@@ -10056,7 +10053,7 @@
         <v>82</v>
       </c>
       <c r="H190" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
@@ -10067,7 +10064,7 @@
         <v>515</v>
       </c>
       <c r="C191" t="s">
-        <v>1261</v>
+        <v>1256</v>
       </c>
       <c r="D191" t="s">
         <v>784</v>
@@ -10082,7 +10079,7 @@
         <v>83</v>
       </c>
       <c r="H191" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
@@ -10093,7 +10090,7 @@
         <v>516</v>
       </c>
       <c r="C192" t="s">
-        <v>1262</v>
+        <v>1257</v>
       </c>
       <c r="D192" t="s">
         <v>787</v>
@@ -10108,7 +10105,7 @@
         <v>84</v>
       </c>
       <c r="H192" t="s">
-        <v>1461</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.2">
@@ -10119,7 +10116,7 @@
         <v>517</v>
       </c>
       <c r="C193" t="s">
-        <v>1263</v>
+        <v>1258</v>
       </c>
       <c r="D193" t="s">
         <v>786</v>
@@ -10134,7 +10131,7 @@
         <v>85</v>
       </c>
       <c r="H193" t="s">
-        <v>1462</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.2">
@@ -10145,7 +10142,7 @@
         <v>518</v>
       </c>
       <c r="C194" t="s">
-        <v>1264</v>
+        <v>1259</v>
       </c>
       <c r="D194" t="s">
         <v>628</v>
@@ -10160,7 +10157,7 @@
         <v>86</v>
       </c>
       <c r="H194" t="s">
-        <v>1463</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.2">
@@ -10171,7 +10168,7 @@
         <v>519</v>
       </c>
       <c r="C195" t="s">
-        <v>1265</v>
+        <v>1260</v>
       </c>
       <c r="D195" t="s">
         <v>783</v>
@@ -10186,7 +10183,7 @@
         <v>87</v>
       </c>
       <c r="H195" t="s">
-        <v>1464</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.2">
@@ -10197,7 +10194,7 @@
         <v>520</v>
       </c>
       <c r="C196" t="s">
-        <v>1266</v>
+        <v>1261</v>
       </c>
       <c r="D196" t="s">
         <v>782</v>
@@ -10212,7 +10209,7 @@
         <v>88</v>
       </c>
       <c r="H196" t="s">
-        <v>1465</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.2">
@@ -10220,7 +10217,7 @@
         <v>294</v>
       </c>
       <c r="C197" t="s">
-        <v>1267</v>
+        <v>1262</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>937</v>
@@ -10246,7 +10243,7 @@
         <v>295</v>
       </c>
       <c r="C198" t="s">
-        <v>1268</v>
+        <v>1263</v>
       </c>
       <c r="D198" t="s">
         <v>547</v>
@@ -10274,7 +10271,7 @@
         <v>296</v>
       </c>
       <c r="C199" t="s">
-        <v>1269</v>
+        <v>1264</v>
       </c>
       <c r="D199" t="s">
         <v>545</v>
@@ -10302,7 +10299,7 @@
         <v>297</v>
       </c>
       <c r="C200" t="s">
-        <v>1270</v>
+        <v>1265</v>
       </c>
       <c r="D200" t="s">
         <v>537</v>
@@ -10330,7 +10327,7 @@
         <v>521</v>
       </c>
       <c r="C201" t="s">
-        <v>1271</v>
+        <v>1266</v>
       </c>
       <c r="D201" t="s">
         <v>935</v>
@@ -10345,7 +10342,7 @@
         <v>93</v>
       </c>
       <c r="H201" t="s">
-        <v>1066</v>
+        <v>1461</v>
       </c>
       <c r="I201" s="4"/>
       <c r="J201" s="4"/>
@@ -10358,7 +10355,7 @@
         <v>522</v>
       </c>
       <c r="C202" t="s">
-        <v>1272</v>
+        <v>1267</v>
       </c>
       <c r="D202" t="s">
         <v>936</v>
@@ -10373,7 +10370,7 @@
         <v>94</v>
       </c>
       <c r="H202" t="s">
-        <v>1065</v>
+        <v>1462</v>
       </c>
       <c r="I202" s="4"/>
       <c r="J202" s="4"/>
@@ -10386,7 +10383,7 @@
         <v>523</v>
       </c>
       <c r="C203" t="s">
-        <v>1273</v>
+        <v>1268</v>
       </c>
       <c r="D203" t="s">
         <v>929</v>
@@ -10400,8 +10397,8 @@
       <c r="G203" t="s">
         <v>95</v>
       </c>
-      <c r="H203" t="s">
-        <v>1067</v>
+      <c r="H203">
+        <v>151</v>
       </c>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.2">
@@ -10412,7 +10409,7 @@
         <v>524</v>
       </c>
       <c r="C204" t="s">
-        <v>1274</v>
+        <v>1269</v>
       </c>
       <c r="D204" t="s">
         <v>927</v>
@@ -10427,7 +10424,7 @@
         <v>96</v>
       </c>
       <c r="H204" t="s">
-        <v>1068</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.2">
@@ -10438,7 +10435,7 @@
         <v>525</v>
       </c>
       <c r="C205" t="s">
-        <v>1275</v>
+        <v>1270</v>
       </c>
       <c r="D205" t="s">
         <v>925</v>
@@ -10453,7 +10450,7 @@
         <v>97</v>
       </c>
       <c r="H205" t="s">
-        <v>1069</v>
+        <v>1464</v>
       </c>
     </row>
   </sheetData>
@@ -10477,15 +10474,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1286</v>
+        <v>1281</v>
       </c>
       <c r="B1" t="s">
-        <v>1294</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>1287</v>
+        <v>1282</v>
       </c>
       <c r="B2">
         <v>22</v>
@@ -10493,7 +10490,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>1288</v>
+        <v>1283</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -10501,7 +10498,7 @@
     </row>
     <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>1289</v>
+        <v>1284</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -10509,7 +10506,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>1290</v>
+        <v>1285</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -10517,7 +10514,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>1293</v>
+        <v>1288</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -10525,7 +10522,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>1297</v>
+        <v>1292</v>
       </c>
       <c r="B7">
         <v>1</v>

</xml_diff>